<commit_message>
add read xl fail
</commit_message>
<xml_diff>
--- a/購入品リスト.xlsx
+++ b/購入品リスト.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kawa_\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kawa_\OneDrive\ドキュメント\python\akizuki_partslist_maker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DD7625-B456-4C40-998F-A0B93F40E7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96D677E-8FED-4E64-B2EE-DC73AFAF7A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{D323307B-543A-4F04-B8AF-8808710F146E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{D323307B-543A-4F04-B8AF-8808710F146E}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="6" r:id="rId1"/>
+    <sheet name="購入品リスト1" sheetId="10" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="12">
   <si>
     <t>SKU</t>
     <phoneticPr fontId="2"/>
@@ -881,8 +882,8 @@
   </sheetPr>
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="117" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -1246,4 +1247,388 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="68" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA53E2EC-817B-4CBB-BB59-9ED87EAD78EC}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:J20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="40" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="67.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.19921875" customWidth="1"/>
+    <col min="7" max="7" width="43.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="21">
+        <f>SUM(E3:E37)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="11">
+        <v>114659</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="12">
+        <v>1</v>
+      </c>
+      <c r="E3" s="13">
+        <f>PRODUCT(C3,D3)</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A4" s="4">
+        <v>129604</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" ref="E4:E20" si="0">PRODUCT(C4,D4)</f>
+        <v>2</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A5" s="4">
+        <v>109848</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A6" s="4"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A7" s="4"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A8" s="4"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A9" s="4"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" s="4"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11" s="4"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" s="4"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A13" s="4"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A14" s="4"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A15" s="4"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A16" s="4"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A17" s="4"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A18" s="4"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A19" s="4"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="8"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="68" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>